<commit_message>
Update PCB files and add schematic image
Updated GERBER, BOM, and CPL files for the Glider sim stick buttons PCB. Added a new schematic image to aid in hardware design and documentation.
</commit_message>
<xml_diff>
--- a/PCB/Glider_sim_stick_buttons/Glider_sim_stick_CPL.xlsx
+++ b/PCB/Glider_sim_stick_buttons/Glider_sim_stick_CPL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="PickAndPlace_PCB1_2026-01-05" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="PickAndPlace_PCB1_2026-01-19" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -64,7 +64,7 @@
     <t>CONN-TH_XH2.54_3PIN</t>
   </si>
   <si>
-    <t>23.368mm</t>
+    <t>23.165mm</t>
   </si>
   <si>
     <t>-34.849mm</t>
@@ -88,13 +88,13 @@
     <t>CONN-TH_XH2.54-2P</t>
   </si>
   <si>
-    <t>15.748mm</t>
+    <t>16.713mm</t>
   </si>
   <si>
     <t>-32.106mm</t>
   </si>
   <si>
-    <t>14.498mm</t>
+    <t>15.463mm</t>
   </si>
   <si>
     <t>SW5</t>
@@ -133,13 +133,13 @@
     <t>COMM-SMD_16P-L22.5-W18.0-P2.54-TL</t>
   </si>
   <si>
-    <t>19.558mm</t>
+    <t>19.863mm</t>
   </si>
   <si>
     <t>-17.018mm</t>
   </si>
   <si>
-    <t>27.559mm</t>
+    <t>27.864mm</t>
   </si>
   <si>
     <t>-8.128mm</t>

</xml_diff>